<commit_message>
first version: search, facets, filters, time slider, watchlist, fly-in
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -80,6 +80,186 @@
   </si>
   <si>
     <t xml:space="preserve">letzte Seite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suchergebnisse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort_by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sortieren nach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">authors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autoren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show_all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alle anzeigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">your_selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ihre Auswahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">journals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeitschriften</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">involved_people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beteiligte Personen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watchlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merkliste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hilfe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transcription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transkription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suchfunktion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_quote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zitat aus der angegebenen Quelle. Zitate spiegeln das Interesse der Bearbeiter/in wieder, sind aber wortwörtliche Übernahmen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_viewer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ansicht des zitierten Beitrags bzw. der zitierten Beiträge  in einem Viewer. Die Digitalisate werden von BnF (Gallica) und der Universitätsbibliothek Heidelberg angeboten und 2021 eingebunden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Titel entspricht dem Werktitel/ der Quelle oder ist vom Projekt vergeben worden, um Abschnitte in Artikeln und Kolumnen zu kennzeichnen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_transcription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Transkription ist eine Beschreibung der aus Sicht des Forschungsprojekts relevanten Inhalte des Beitrags. Die Transktiptionen sind somit Inhaltswiedergaben und/oder Interpretationen der Bearbeiter/innen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alle in der Quelle genannten Personen, meist in der Schreibweise des Quelltextes. Die Personen wurden durch die Bearbeiter/innen erfasst. 2021 wurden sie soweit möglich mit Normdaten referenziert (mehr...).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_text_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klassifizierung des Texttyps durch die Bearbeiter/in. Insgesamt wurden ## Textarten herausgestellt, davon ## französischsprachig, ## deutschsprachig.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stichpunkte, mit denen die jeweilige Bearbeiter/in markiert hat, welche für das Forschungsprojekt interessanten Themenbereiche im Beitrag behandelt werden. Die Angabe von Themen ergänzen oder ersetzen auch die Beschreibung.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">help_search_feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektbalken ermöglicht neben der Suche in allen Datenbanken auch die separate Auswahl einer einzelnen und macht die ursprünglichen Zugehörigkeiten sichtbar.
+Die Volltextsuche fragt alle Informationen ab und beeinflusst die Filtervorschläge.
+Der Zeitbalken grnezt nach Erscheinungsdatum ein; Achtung: für die Jahre 1941-1944 wurden keine Daten erhoben.
+Personen, Autoren, Zeitschriften, Bucheinträge...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datamodel_and_data_curation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datenmodell &amp; Anreicherung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publikationen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reuse_question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reuse?</t>
   </si>
 </sst>
 </file>
@@ -154,9 +334,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -176,27 +360,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -210,7 +394,7 @@
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -224,7 +408,7 @@
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -232,7 +416,7 @@
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -240,7 +424,7 @@
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -248,7 +432,7 @@
       <c r="A6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -256,7 +440,7 @@
       <c r="A7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -264,8 +448,251 @@
       <c r="A8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="75.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="181.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
metadata for single view
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -260,6 +260,24 @@
   </si>
   <si>
     <t xml:space="preserve">Reuse?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description_comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschreibung / Kommentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project_affiliation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektzugehörigkeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citation_format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empfohlene Zitation</t>
   </si>
 </sst>
 </file>
@@ -360,15 +378,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
@@ -695,6 +713,30 @@
         <v>78</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
adds watchlist to search form
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -278,6 +278,24 @@
   </si>
   <si>
     <t xml:space="preserve">empfohlene Zitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watchlist_only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nur Einträge in der Merkliste anzeigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einträge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eintrag</t>
   </si>
 </sst>
 </file>
@@ -378,15 +396,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
@@ -737,6 +755,30 @@
         <v>84</v>
       </c>
     </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
range control: horiz scaler updated on critieria change
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t xml:space="preserve">aus dem Quelltext erfasste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty_watchlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merkliste leeren</t>
   </si>
 </sst>
 </file>
@@ -420,15 +426,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
@@ -835,6 +841,14 @@
         <v>98</v>
       </c>
     </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
adds wikidata data points
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -326,6 +326,42 @@
   </si>
   <si>
     <t xml:space="preserve">Merkliste leeren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">person_details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personendetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">authority_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normdatenverknüpfung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_wikidata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aus Wikidata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">born</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geboren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">died</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verstorben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">journal_details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quellendetails</t>
   </si>
 </sst>
 </file>
@@ -426,15 +462,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+      <selection pane="bottomLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
@@ -849,6 +885,54 @@
         <v>100</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
adds printing, json rendering, smaller fixes
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -362,6 +362,18 @@
   </si>
   <si>
     <t xml:space="preserve">Quellendetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source_wikidata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data</t>
   </si>
 </sst>
 </file>
@@ -462,15 +474,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
+      <selection pane="bottomLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
@@ -933,6 +945,36 @@
         <v>112</v>
       </c>
     </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
adds multi-printer and some translations
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -477,15 +477,15 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+      <selection pane="bottomLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.28"/>
   </cols>

</xml_diff>

<commit_message>
adds message for print limit
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t xml:space="preserve">data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print_too_many_results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ihre Suchanfrage liefert zu viele Resultate, die Druckfunktion steht nur für bis zu 100 Einträge zur Verfügung</t>
   </si>
 </sst>
 </file>
@@ -474,15 +480,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.45"/>
@@ -975,6 +981,14 @@
         <v>116</v>
       </c>
     </row>
+    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
improves #2059, #2061, #2063, #2054
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="123">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">Datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autor</t>
   </si>
   <si>
     <t xml:space="preserve">authors</t>
@@ -380,6 +386,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ihre Suchanfrage liefert zu viele Resultate, die Druckfunktion steht nur für bis zu 100 Einträge zur Verfügung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zurücksetzen</t>
   </si>
 </sst>
 </file>
@@ -480,15 +492,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
+      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.45"/>
@@ -646,15 +658,15 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>40</v>
@@ -683,9 +695,6 @@
       <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -694,6 +703,9 @@
       <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C23" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -727,7 +739,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>57</v>
       </c>
@@ -735,7 +747,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>59</v>
       </c>
@@ -743,7 +755,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>61</v>
       </c>
@@ -751,7 +763,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>63</v>
       </c>
@@ -767,7 +779,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>67</v>
       </c>
@@ -775,7 +787,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="75.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>69</v>
       </c>
@@ -783,7 +795,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="181.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="75.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>71</v>
       </c>
@@ -791,7 +803,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="181.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>73</v>
       </c>
@@ -863,7 +875,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>91</v>
       </c>
@@ -871,7 +883,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>93</v>
       </c>
@@ -879,7 +891,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>95</v>
       </c>
@@ -887,7 +899,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>97</v>
       </c>
@@ -956,21 +968,15 @@
         <v>113</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,15 +984,37 @@
         <v>116</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes #2060, #2067, #2073, #2074, #2076, 2077, #2078, #2079, #2080
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="124">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -271,13 +271,13 @@
     <t xml:space="preserve">description_comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Beschreibung / Kommentar</t>
+    <t xml:space="preserve">Kommentar</t>
   </si>
   <si>
     <t xml:space="preserve">project_affiliation</t>
   </si>
   <si>
-    <t xml:space="preserve">Projektzugehörigkeit</t>
+    <t xml:space="preserve">Projekt</t>
   </si>
   <si>
     <t xml:space="preserve">citation_format</t>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t xml:space="preserve">zurücksetzen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project</t>
   </si>
 </sst>
 </file>
@@ -492,15 +495,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.45"/>
@@ -1017,6 +1018,14 @@
         <v>122</v>
       </c>
     </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixes #2085, #2096, #2087, #2095
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="135">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -404,6 +404,30 @@
   </si>
   <si>
     <t xml:space="preserve">Weitere in der Datenbank vorkommende Schreibweise / Benennung:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_involved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_creator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_journal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeitschrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expand_all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alle ausklappen</t>
   </si>
 </sst>
 </file>
@@ -504,15 +528,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
+      <selection pane="bottomLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.45"/>
@@ -1049,6 +1073,46 @@
         <v>126</v>
       </c>
     </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixes #2006, #2096, #2106
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="139">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -428,6 +428,18 @@
   </si>
   <si>
     <t xml:space="preserve">alle ausklappen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contribution_type_journal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeitschriftenbeitrag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contribution_type_book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buchbeitrag</t>
   </si>
 </sst>
 </file>
@@ -528,15 +540,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+      <selection pane="bottomLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.45"/>
@@ -1113,6 +1125,22 @@
         <v>134</v>
       </c>
     </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
cleaning up & facets
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="238">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -744,6 +744,42 @@
   </si>
   <si>
     <t xml:space="preserve">your selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normdatenbank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normdatenbanken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OwnReality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palais Beauharnais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfkv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFKV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wikidata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wikdata</t>
   </si>
 </sst>
 </file>
@@ -881,10 +917,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ73"/>
+  <dimension ref="A1:AMJ79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1870,6 +1906,54 @@
         <v>225</v>
       </c>
     </row>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
copy from dev branch, cleanup
</commit_message>
<xml_diff>
--- a/data/translations.xlsx
+++ b/data/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="227">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">text type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_person_id</t>
   </si>
   <si>
     <t xml:space="preserve">filters</t>
@@ -839,28 +842,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -877,14 +884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ73"/>
+  <dimension ref="A1:AMJ74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -892,7 +899,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="30.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="30.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="5" style="1" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,13 +1023,13 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1058,13 +1065,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1106,7 +1113,7 @@
       <c r="B16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1187,190 +1194,181 @@
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="157.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="D27" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="157.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" s="4" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="4" t="s">
+    </row>
+    <row r="29" s="5" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="AMH28" s="0"/>
-      <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="2"/>
+      <c r="AMH29" s="3"/>
+      <c r="AMI29" s="3"/>
+      <c r="AMJ29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="4" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="B31" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="1" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="1" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="4" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="B36" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,76 +1376,76 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="C38" s="1" t="s">
-        <v>119</v>
+        <v>4</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>120</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="4" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="C40" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="D40" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="4" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="4" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="C42" s="5" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1456,376 +1454,376 @@
         <v>132</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>141</v>
+      <c r="B46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="280.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="C49" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B49" s="1" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="280.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B50" s="1" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="4" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="C52" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B52" s="1" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="D53" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="D55" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C55" s="5" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>170</v>
+      <c r="C56" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="D57" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="D58" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>182</v>
+      <c r="D60" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>207</v>
+        <v>80</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>205</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="D68" s="2" t="s">
-        <v>69</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="D69" s="2" t="s">
-        <v>211</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D70" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,41 +1831,55 @@
         <v>215</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>217</v>
+        <v>40</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="D72" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="D73" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B73" s="1" t="s">
+    </row>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>225</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>